<commit_message>
Item Generation and Stat point spending - changed inventory size to match the character display, player now starts off with a little less slots but can expand by buying more - added Stat point spending system - player now gets some random base stat increase on level up - added basic item generation code, still work in progress
</commit_message>
<xml_diff>
--- a/data/content/Items.xlsx
+++ b/data/content/Items.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\EndlessBattleFC\data\content\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="18000" windowHeight="20820"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="18000" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="ItemSlots" sheetId="1" r:id="rId1"/>
+    <sheet name="ItemRarity" sheetId="2" r:id="rId2"/>
+    <sheet name="ItemUniques" sheetId="4" r:id="rId3"/>
+    <sheet name="ItemSets" sheetId="3" r:id="rId4"/>
+    <sheet name="ItemSetStats" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -47,27 +46,9 @@
     <t>shoulder</t>
   </si>
   <si>
-    <t>weapon</t>
-  </si>
-  <si>
-    <t>offhand</t>
-  </si>
-  <si>
     <t>neck</t>
   </si>
   <si>
-    <t>ring1</t>
-  </si>
-  <si>
-    <t>ring2</t>
-  </si>
-  <si>
-    <t>trinket1</t>
-  </si>
-  <si>
-    <t>trinket2</t>
-  </si>
-  <si>
     <t>wrist</t>
   </si>
   <si>
@@ -101,9 +82,6 @@
     <t>Hands</t>
   </si>
   <si>
-    <t>Weapon</t>
-  </si>
-  <si>
     <t>Offhand</t>
   </si>
   <si>
@@ -114,6 +92,150 @@
   </si>
   <si>
     <t>Trinket</t>
+  </si>
+  <si>
+    <t>common</t>
+  </si>
+  <si>
+    <t>uncommon</t>
+  </si>
+  <si>
+    <t>rare</t>
+  </si>
+  <si>
+    <t>poor</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>magic</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Uncommon</t>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>multiplier</t>
+  </si>
+  <si>
+    <t>dropChance</t>
+  </si>
+  <si>
+    <t>secondaryStatRolls</t>
+  </si>
+  <si>
+    <t>maxSockets</t>
+  </si>
+  <si>
+    <t>socketRolls</t>
+  </si>
+  <si>
+    <t>mainHand</t>
+  </si>
+  <si>
+    <t>offHand</t>
+  </si>
+  <si>
+    <t>Mainhand</t>
+  </si>
+  <si>
+    <t>endlessGarment</t>
+  </si>
+  <si>
+    <t>Endless Garments</t>
+  </si>
+  <si>
+    <t>slot</t>
+  </si>
+  <si>
+    <t>requiredItems</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>agi</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>vit</t>
+  </si>
+  <si>
+    <t>requiredLevel</t>
+  </si>
+  <si>
+    <t>xpMult</t>
+  </si>
+  <si>
+    <t>goldMult</t>
+  </si>
+  <si>
+    <t>The Beater</t>
+  </si>
+  <si>
+    <t>mhBeater</t>
+  </si>
+  <si>
+    <t>spd</t>
+  </si>
+  <si>
+    <t>endlessGarment1</t>
+  </si>
+  <si>
+    <t>slot1</t>
+  </si>
+  <si>
+    <t>slot2</t>
+  </si>
+  <si>
+    <t>slot3</t>
+  </si>
+  <si>
+    <t>slot4</t>
+  </si>
+  <si>
+    <t>slot5</t>
+  </si>
+  <si>
+    <t>slot6</t>
+  </si>
+  <si>
+    <t>slot7</t>
+  </si>
+  <si>
+    <t>slot8</t>
+  </si>
+  <si>
+    <t>ring</t>
+  </si>
+  <si>
+    <t>trinket</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -423,7 +545,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -431,143 +553,597 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>0.8</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.8</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>1.2</v>
+      </c>
+      <c r="D4">
+        <v>0.4</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>1.4</v>
+      </c>
+      <c r="D5">
+        <v>0.12</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>1.9</v>
+      </c>
+      <c r="D6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>2.7</v>
+      </c>
+      <c r="D7">
+        <v>0.01</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8">
+        <v>3.5</v>
+      </c>
+      <c r="D8">
+        <v>1E-3</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>0.8</v>
+      </c>
+      <c r="E2">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I3">
+        <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small item update - added placeholder icons for the item types - init script now recognizes being run in node / browser
</commit_message>
<xml_diff>
--- a/data/content/Items.xlsx
+++ b/data/content/Items.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\EndlessBattleFC\data\content\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="7"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="ItemSlots" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="ItemRarity" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="ItemUniques" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="ItemSets" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="ItemSetStats" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="ItemSuffix" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="ItemPrefix" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="WeaponTypes" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="ArmorTypes" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="ItemSlots" sheetId="1" r:id="rId1"/>
+    <sheet name="ItemRarity" sheetId="2" r:id="rId2"/>
+    <sheet name="ItemUniques" sheetId="3" r:id="rId3"/>
+    <sheet name="ItemSets" sheetId="4" r:id="rId4"/>
+    <sheet name="ItemSetStats" sheetId="5" r:id="rId5"/>
+    <sheet name="ItemSuffix" sheetId="6" r:id="rId6"/>
+    <sheet name="ItemPrefix" sheetId="7" r:id="rId7"/>
+    <sheet name="WeaponTypes" sheetId="8" r:id="rId8"/>
+    <sheet name="ArmorTypes" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -1129,32 +1134,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1166,7 +1153,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1174,2490 +1161,2651 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.4642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="10.42578125"/>
+    <col min="2" max="2" width="10.28515625"/>
+    <col min="3" max="3" width="11.42578125"/>
+    <col min="4" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>6</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9948979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="12.28515625"/>
+    <col min="2" max="2" width="8.7109375"/>
+    <col min="3" max="3" width="13.28515625"/>
+    <col min="4" max="4" width="11.5703125"/>
+    <col min="5" max="5" width="18"/>
+    <col min="6" max="6" width="11"/>
+    <col min="7" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>0.8</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>0.8</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4">
         <v>1.2</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4">
         <v>0.4</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5">
         <v>1.4</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5">
         <v>0.12</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6">
         <v>1.9</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="E6" s="0" t="n">
+      <c r="D6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E6">
         <v>3</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7">
         <v>2.7</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7">
         <v>0.01</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7">
         <v>4</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8">
         <v>3.5</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="E8" s="0" t="n">
+      <c r="D8">
+        <v>1E-3</v>
+      </c>
+      <c r="E8">
         <v>6</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.70918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.5765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="9.7109375"/>
+    <col min="2" max="2" width="10.5703125"/>
+    <col min="3" max="3" width="10"/>
+    <col min="4" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>0.8</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="6.85714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.85714285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="5.28061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="15.7109375"/>
+    <col min="2" max="2" width="16.85546875"/>
+    <col min="3" max="3" width="11"/>
+    <col min="4" max="4" width="13.5703125"/>
+    <col min="5" max="5" width="13.85546875"/>
+    <col min="6" max="8" width="6.85546875"/>
+    <col min="9" max="9" width="8.85546875"/>
+    <col min="10" max="10" width="10"/>
+    <col min="11" max="11" width="5.28515625"/>
+    <col min="12" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2">
         <v>5</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="16.7109375"/>
+    <col min="2" max="2" width="15.7109375"/>
+    <col min="3" max="3" width="13.85546875"/>
+    <col min="4" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>10</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3">
         <v>4</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>1.1</v>
+      <c r="H3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I3">
+        <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A140"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="15.42578125"/>
+    <col min="2" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>209</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A120"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="16.7109375"/>
+    <col min="2" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>329</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.72959183673469"/>
+    <col min="1" max="2" width="8.7109375"/>
+    <col min="3" max="3" width="15"/>
+    <col min="4" max="4" width="13.42578125"/>
+    <col min="5" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>330</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>331</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>332</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>334</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>335</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="C2" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D2" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>337</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>338</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="C3" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D3" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>339</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>340</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="C4" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>342</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="0" t="s">
+      <c r="C5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>343</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>344</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="C6" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E6" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>345</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>346</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="0" t="s">
+      <c r="C7" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D7" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>347</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>348</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="C8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>349</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>350</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="C9" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>351</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>352</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F10" s="0" t="s">
+      <c r="E10" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>353</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>354</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="C11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>355</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>356</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="C12" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>357</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>358</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F13" s="0" t="s">
+      <c r="C13" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>359</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="D14" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>362</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>363</v>
       </c>
-      <c r="D15" s="0" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F15" s="0" t="s">
+      <c r="D15" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
         <v>361</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Item Update - Item Stats are now applied on equip - Inventory reacts to changes in the storage slots, still glitched with the background icon - Item Tooltips shows very basic stat info, needs to be expanded - Fixed hand slot spelling in data
</commit_message>
<xml_diff>
--- a/data/content/Items.xlsx
+++ b/data/content/Items.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986" activeTab="8"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="ItemSlots" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>Wrists</t>
   </si>
   <si>
-    <t>hand</t>
-  </si>
-  <si>
     <t>Hands</t>
   </si>
   <si>
@@ -1129,6 +1126,9 @@
   </si>
   <si>
     <t>Amulet</t>
+  </si>
+  <si>
+    <t>hands</t>
   </si>
 </sst>
 </file>
@@ -1448,11 +1448,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,10 +1547,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>366</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1558,10 +1558,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -1569,10 +1569,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1580,10 +1580,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1591,10 +1591,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1633,24 +1633,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
       </c>
       <c r="C2">
         <v>0.8</v>
@@ -1667,10 +1667,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1687,10 +1687,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
         <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
       </c>
       <c r="C4">
         <v>1.2</v>
@@ -1707,10 +1707,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
         <v>37</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
       </c>
       <c r="C5">
         <v>1.4</v>
@@ -1727,10 +1727,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
         <v>39</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
       </c>
       <c r="C6">
         <v>1.9</v>
@@ -1747,10 +1747,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
         <v>41</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
       </c>
       <c r="C7">
         <v>2.7</v>
@@ -1767,10 +1767,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
         <v>43</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
       </c>
       <c r="C8">
         <v>3.5</v>
@@ -1818,30 +1818,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
       </c>
       <c r="E2">
         <v>0.8</v>
@@ -1889,42 +1889,42 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>58</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>59</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>60</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>61</v>
-      </c>
-      <c r="L1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -1945,13 +1945,13 @@
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1981,36 +1981,36 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
         <v>65</v>
       </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>66</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>69</v>
-      </c>
-      <c r="I1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -2030,10 +2030,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -2070,702 +2070,702 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2793,602 +2793,602 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -3424,24 +3424,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D1" t="s">
         <v>330</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>331</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>332</v>
-      </c>
-      <c r="F1" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B2" t="s">
         <v>334</v>
-      </c>
-      <c r="B2" t="s">
-        <v>335</v>
       </c>
       <c r="C2" t="b">
         <f>TRUE()</f>
@@ -3452,15 +3452,15 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" t="s">
         <v>337</v>
-      </c>
-      <c r="B3" t="s">
-        <v>338</v>
       </c>
       <c r="C3" t="b">
         <f>TRUE()</f>
@@ -3471,15 +3471,15 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B4" t="s">
         <v>339</v>
-      </c>
-      <c r="B4" t="s">
-        <v>340</v>
       </c>
       <c r="C4" t="b">
         <f>TRUE()</f>
@@ -3490,15 +3490,15 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C5" t="b">
         <f>TRUE()</f>
@@ -3509,15 +3509,15 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>342</v>
+      </c>
+      <c r="B6" t="s">
         <v>343</v>
-      </c>
-      <c r="B6" t="s">
-        <v>344</v>
       </c>
       <c r="C6" t="b">
         <f>TRUE()</f>
@@ -3528,15 +3528,15 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>344</v>
+      </c>
+      <c r="B7" t="s">
         <v>345</v>
-      </c>
-      <c r="B7" t="s">
-        <v>346</v>
       </c>
       <c r="C7" t="b">
         <f>TRUE()</f>
@@ -3547,15 +3547,15 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B8" t="s">
         <v>347</v>
-      </c>
-      <c r="B8" t="s">
-        <v>348</v>
       </c>
       <c r="C8" t="b">
         <f>TRUE()</f>
@@ -3566,45 +3566,45 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B9" t="s">
         <v>349</v>
-      </c>
-      <c r="B9" t="s">
-        <v>350</v>
       </c>
       <c r="C9" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>350</v>
+      </c>
+      <c r="B10" t="s">
         <v>351</v>
-      </c>
-      <c r="B10" t="s">
-        <v>352</v>
       </c>
       <c r="E10" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>352</v>
+      </c>
+      <c r="B11" t="s">
         <v>353</v>
-      </c>
-      <c r="B11" t="s">
-        <v>354</v>
       </c>
       <c r="C11" t="b">
         <f>TRUE()</f>
@@ -3615,15 +3615,15 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>354</v>
+      </c>
+      <c r="B12" t="s">
         <v>355</v>
-      </c>
-      <c r="B12" t="s">
-        <v>356</v>
       </c>
       <c r="C12" t="b">
         <f>TRUE()</f>
@@ -3634,15 +3634,15 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>356</v>
+      </c>
+      <c r="B13" t="s">
         <v>357</v>
-      </c>
-      <c r="B13" t="s">
-        <v>358</v>
       </c>
       <c r="C13" t="b">
         <f>TRUE()</f>
@@ -3653,37 +3653,37 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>358</v>
+      </c>
+      <c r="B14" t="s">
         <v>359</v>
-      </c>
-      <c r="B14" t="s">
-        <v>360</v>
       </c>
       <c r="D14" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>361</v>
+      </c>
+      <c r="B15" t="s">
         <v>362</v>
-      </c>
-      <c r="B15" t="s">
-        <v>363</v>
       </c>
       <c r="D15" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3696,11 +3696,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3737,7 +3737,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3753,7 +3753,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3774,34 +3774,34 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>366</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>